<commit_message>
Allow removing tweets with 'commenting' SDQC labels from data load
</commit_message>
<xml_diff>
--- a/src/performance_testing/dastpheme_performance.xlsx
+++ b/src/performance_testing/dastpheme_performance.xlsx
@@ -782,22 +782,22 @@
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>pheme_ts</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>dastpheme_ts</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>dast_ts</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>pheme_ts</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>dastpheme_ts</c:v>
-                </c:pt>
                 <c:pt idx="3">
+                  <c:v>pheme_nts</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>dastpheme_nts</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>dast_nts</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>pheme_nts</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>dastpheme_nts</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -809,22 +809,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.56000000000000005</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.44</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.44</c:v>
+                  <c:v>0.53</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.56999999999999995</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.43</c:v>
+                  <c:v>0.52</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.47</c:v>
+                  <c:v>0.52</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -919,22 +919,22 @@
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>pheme_ts</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>dastpheme_ts</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>dast_ts</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>pheme_ts</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>dastpheme_ts</c:v>
-                </c:pt>
                 <c:pt idx="3">
+                  <c:v>pheme_nts</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>dastpheme_nts</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>dast_nts</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>pheme_nts</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>dastpheme_nts</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -946,22 +946,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.76</c:v>
+                  <c:v>0.67</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.6</c:v>
+                  <c:v>0.68</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.6</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.79</c:v>
+                  <c:v>0.67</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.6</c:v>
+                  <c:v>0.77</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.68</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -977,11 +977,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="437656752"/>
-        <c:axId val="437657144"/>
+        <c:axId val="608985448"/>
+        <c:axId val="608989368"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="437656752"/>
+        <c:axId val="608985448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1024,7 +1024,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="437657144"/>
+        <c:crossAx val="608989368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1032,7 +1032,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="437657144"/>
+        <c:axId val="608989368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1083,7 +1083,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="437656752"/>
+        <c:crossAx val="608985448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1204,7 +1204,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1305,7 +1304,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1449,7 +1447,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1539,11 +1536,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="565292664"/>
-        <c:axId val="565288744"/>
+        <c:axId val="609002696"/>
+        <c:axId val="609003088"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="565292664"/>
+        <c:axId val="609002696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1586,7 +1583,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="565288744"/>
+        <c:crossAx val="609003088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1594,7 +1591,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="565288744"/>
+        <c:axId val="609003088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1645,7 +1642,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="565292664"/>
+        <c:crossAx val="609002696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1659,7 +1656,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1766,7 +1762,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1867,7 +1862,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2011,7 +2005,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2101,11 +2094,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="565293448"/>
-        <c:axId val="565293056"/>
+        <c:axId val="609004264"/>
+        <c:axId val="609001128"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="565293448"/>
+        <c:axId val="609004264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2148,7 +2141,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="565293056"/>
+        <c:crossAx val="609001128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2156,7 +2149,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="565293056"/>
+        <c:axId val="609001128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2207,7 +2200,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="565293448"/>
+        <c:crossAx val="609004264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2221,7 +2214,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2328,7 +2320,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2429,7 +2420,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2573,7 +2563,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2663,11 +2652,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="565289136"/>
-        <c:axId val="565293840"/>
+        <c:axId val="609001520"/>
+        <c:axId val="609002304"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="565289136"/>
+        <c:axId val="609001520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2710,7 +2699,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="565293840"/>
+        <c:crossAx val="609002304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2718,7 +2707,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="565293840"/>
+        <c:axId val="609002304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2769,7 +2758,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="565289136"/>
+        <c:crossAx val="609001520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2783,7 +2772,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2890,7 +2878,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2991,7 +2978,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -3135,7 +3121,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -3225,11 +3210,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="565289528"/>
-        <c:axId val="391913944"/>
+        <c:axId val="608997992"/>
+        <c:axId val="608999560"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="565289528"/>
+        <c:axId val="608997992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3272,7 +3257,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="391913944"/>
+        <c:crossAx val="608999560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3280,7 +3265,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="391913944"/>
+        <c:axId val="608999560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3331,7 +3316,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="565289528"/>
+        <c:crossAx val="608997992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3345,7 +3330,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3497,7 +3481,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -3634,7 +3617,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -3717,11 +3699,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="391915512"/>
-        <c:axId val="391911984"/>
+        <c:axId val="609001912"/>
+        <c:axId val="608999952"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="391915512"/>
+        <c:axId val="609001912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3764,7 +3746,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="391911984"/>
+        <c:crossAx val="608999952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3772,7 +3754,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="391911984"/>
+        <c:axId val="608999952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3823,7 +3805,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="391915512"/>
+        <c:crossAx val="609001912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3837,7 +3819,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4080,22 +4061,22 @@
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>pheme_ts</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>dastpheme_ts</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>dast_ts</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>pheme_ts</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>dastpheme_ts</c:v>
-                </c:pt>
                 <c:pt idx="3">
+                  <c:v>pheme_nts</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>dastpheme_nts</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>dast_nts</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>pheme_nts</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>dastpheme_nts</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4107,19 +4088,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>0.46</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.48</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>0.47</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.46</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.52</c:v>
-                </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.54</c:v>
+                  <c:v>0.47</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.43</c:v>
+                  <c:v>0.49</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.49</c:v>
@@ -4217,22 +4198,22 @@
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>pheme_ts</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>dastpheme_ts</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>dast_ts</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>pheme_ts</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>dastpheme_ts</c:v>
-                </c:pt>
                 <c:pt idx="3">
+                  <c:v>pheme_nts</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>dastpheme_nts</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>dast_nts</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>pheme_nts</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>dastpheme_nts</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4244,22 +4225,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.81</c:v>
+                  <c:v>0.79</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.84</c:v>
+                  <c:v>0.77</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.79</c:v>
+                  <c:v>0.77</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.79</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.77</c:v>
+                  <c:v>0.74</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.73</c:v>
+                  <c:v>0.76</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4275,11 +4256,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="437664200"/>
-        <c:axId val="437663416"/>
+        <c:axId val="608990544"/>
+        <c:axId val="608992896"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="437664200"/>
+        <c:axId val="608990544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4322,7 +4303,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="437663416"/>
+        <c:crossAx val="608992896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4330,7 +4311,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="437663416"/>
+        <c:axId val="608992896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4381,7 +4362,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="437664200"/>
+        <c:crossAx val="608990544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4638,22 +4619,22 @@
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>pheme_ts</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>dastpheme_ts</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>dast_ts</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>pheme_ts</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>dastpheme_ts</c:v>
-                </c:pt>
                 <c:pt idx="3">
+                  <c:v>pheme_nts</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>dastpheme_nts</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>dast_nts</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>pheme_nts</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>dastpheme_nts</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4665,22 +4646,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.5</c:v>
+                  <c:v>0.44</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.43</c:v>
+                  <c:v>0.46</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.47</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.48</c:v>
+                  <c:v>0.45</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.42</c:v>
+                  <c:v>0.46</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.48</c:v>
+                  <c:v>0.46</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4775,22 +4756,22 @@
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>pheme_ts</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>dastpheme_ts</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>dast_ts</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>pheme_ts</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>dastpheme_ts</c:v>
-                </c:pt>
                 <c:pt idx="3">
+                  <c:v>pheme_nts</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>dastpheme_nts</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>dast_nts</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>pheme_nts</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>dastpheme_nts</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4802,22 +4783,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>0.77</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>0.76</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
+                  <c:v>0.76</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.77</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>0.75</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.73</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.73</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.74</c:v>
-                </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.72</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4833,11 +4814,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="437661456"/>
-        <c:axId val="437657928"/>
+        <c:axId val="608995640"/>
+        <c:axId val="608988976"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="437661456"/>
+        <c:axId val="608995640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4880,7 +4861,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="437657928"/>
+        <c:crossAx val="608988976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4888,7 +4869,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="437657928"/>
+        <c:axId val="608988976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4939,7 +4920,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="437661456"/>
+        <c:crossAx val="608995640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5196,22 +5177,22 @@
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>pheme_ts</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>dastpheme_ts</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>dast_ts</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>pheme_ts</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>dastpheme_ts</c:v>
-                </c:pt>
                 <c:pt idx="3">
+                  <c:v>pheme_nts</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>dastpheme_nts</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>dast_nts</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>pheme_nts</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>dastpheme_nts</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5223,22 +5204,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>0.46</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>0.45</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.47</c:v>
-                </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.46</c:v>
+                  <c:v>0.45</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.45</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.45</c:v>
+                  <c:v>0.46</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5333,22 +5314,22 @@
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>pheme_ts</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>dastpheme_ts</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>dast_ts</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>pheme_ts</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>dastpheme_ts</c:v>
-                </c:pt>
                 <c:pt idx="3">
+                  <c:v>pheme_nts</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>dastpheme_nts</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>dast_nts</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>pheme_nts</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>dastpheme_nts</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5360,22 +5341,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>0.82</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>0.81</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>0.82</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.8</c:v>
-                </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.8</c:v>
+                  <c:v>0.83</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.82</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.8</c:v>
+                  <c:v>0.82</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5391,11 +5372,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="437658712"/>
-        <c:axId val="437659104"/>
+        <c:axId val="608994856"/>
+        <c:axId val="608994072"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="437658712"/>
+        <c:axId val="608994856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5438,7 +5419,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="437659104"/>
+        <c:crossAx val="608994072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5446,7 +5427,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="437659104"/>
+        <c:axId val="608994072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5497,7 +5478,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="437658712"/>
+        <c:crossAx val="608994856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5754,22 +5735,22 @@
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>pheme_ts</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>dastpheme_ts</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>dast_ts</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>pheme_ts</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>dastpheme_ts</c:v>
-                </c:pt>
                 <c:pt idx="3">
+                  <c:v>pheme_nts</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>dastpheme_nts</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>dast_nts</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>pheme_nts</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>dastpheme_nts</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5781,22 +5762,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.53</c:v>
+                  <c:v>0.47</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0.48</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.46</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>0.44</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.51</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.5</c:v>
-                </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.44</c:v>
+                  <c:v>0.52</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.56999999999999995</c:v>
+                  <c:v>0.49</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5891,22 +5872,22 @@
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>pheme_ts</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>dastpheme_ts</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>dast_ts</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>pheme_ts</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>dastpheme_ts</c:v>
-                </c:pt>
                 <c:pt idx="3">
+                  <c:v>pheme_nts</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>dastpheme_nts</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>dast_nts</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>pheme_nts</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>dastpheme_nts</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5918,19 +5899,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>0.79</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.78</c:v>
-                </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.77</c:v>
+                  <c:v>0.79</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.78</c:v>
+                  <c:v>0.79</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.78</c:v>
+                  <c:v>0.79</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.79</c:v>
@@ -5949,11 +5930,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="437659496"/>
-        <c:axId val="437660672"/>
+        <c:axId val="608997600"/>
+        <c:axId val="608986232"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="437659496"/>
+        <c:axId val="608997600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5996,7 +5977,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="437660672"/>
+        <c:crossAx val="608986232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6004,7 +5985,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="437660672"/>
+        <c:axId val="608986232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6055,7 +6036,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="437659496"/>
+        <c:crossAx val="608997600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6312,22 +6293,22 @@
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>pheme_ts</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>dastpheme_ts</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>dast_ts</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>pheme_ts</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>dastpheme_ts</c:v>
-                </c:pt>
                 <c:pt idx="3">
+                  <c:v>pheme_nts</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>dastpheme_nts</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>dast_nts</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>pheme_nts</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>dastpheme_nts</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6342,19 +6323,19 @@
                   <c:v>0.44</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0.43</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>0.44</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.43</c:v>
-                </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.43</c:v>
+                  <c:v>0.44</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.44</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.43</c:v>
+                  <c:v>0.44</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6449,22 +6430,22 @@
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>pheme_ts</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>dastpheme_ts</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>dast_ts</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>pheme_ts</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>dastpheme_ts</c:v>
-                </c:pt>
                 <c:pt idx="3">
+                  <c:v>pheme_nts</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>dastpheme_nts</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>dast_nts</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>pheme_nts</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>dastpheme_nts</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6479,19 +6460,19 @@
                   <c:v>0.78</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.78</c:v>
+                  <c:v>0.77</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.76</c:v>
+                  <c:v>0.79</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.76</c:v>
+                  <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.78</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.76</c:v>
+                  <c:v>0.79</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6507,11 +6488,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="437661064"/>
-        <c:axId val="437661848"/>
+        <c:axId val="608986624"/>
+        <c:axId val="608987016"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="437661064"/>
+        <c:axId val="608986624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6554,7 +6535,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="437661848"/>
+        <c:crossAx val="608987016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6562,7 +6543,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="437661848"/>
+        <c:axId val="608987016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6613,7 +6594,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="437661064"/>
+        <c:crossAx val="608986624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6870,22 +6851,22 @@
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>pheme_ts</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>dastpheme_ts</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>dast_ts</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>pheme_ts</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>dastpheme_ts</c:v>
-                </c:pt>
                 <c:pt idx="3">
+                  <c:v>pheme_nts</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>dastpheme_nts</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>dast_nts</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>pheme_nts</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>dastpheme_nts</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6897,22 +6878,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.42</c:v>
+                  <c:v>0.45</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.42</c:v>
+                  <c:v>0.44</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.42</c:v>
+                  <c:v>0.45</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.42</c:v>
+                  <c:v>0.44</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.42</c:v>
+                  <c:v>0.44</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.42</c:v>
+                  <c:v>0.44</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7007,22 +6988,22 @@
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>pheme_ts</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>dastpheme_ts</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>dast_ts</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>pheme_ts</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>dastpheme_ts</c:v>
-                </c:pt>
                 <c:pt idx="3">
+                  <c:v>pheme_nts</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>dastpheme_nts</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>dast_nts</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>pheme_nts</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>dastpheme_nts</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -7034,22 +7015,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.71</c:v>
+                  <c:v>0.81</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.71</c:v>
+                  <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.71</c:v>
+                  <c:v>0.81</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.71</c:v>
+                  <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.71</c:v>
+                  <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.71</c:v>
+                  <c:v>0.8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7065,11 +7046,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="437662632"/>
-        <c:axId val="565288352"/>
+        <c:axId val="608987408"/>
+        <c:axId val="608997208"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="437662632"/>
+        <c:axId val="608987408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7112,7 +7093,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="565288352"/>
+        <c:crossAx val="608997208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7120,7 +7101,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="565288352"/>
+        <c:axId val="608997208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7171,7 +7152,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="437662632"/>
+        <c:crossAx val="608987408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7292,7 +7273,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7393,7 +7373,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -7537,7 +7516,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -7627,11 +7605,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="565290312"/>
-        <c:axId val="565294624"/>
+        <c:axId val="608992112"/>
+        <c:axId val="608988192"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="565290312"/>
+        <c:axId val="608992112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7674,7 +7652,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="565294624"/>
+        <c:crossAx val="608988192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7682,7 +7660,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="565294624"/>
+        <c:axId val="608988192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7733,7 +7711,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="565290312"/>
+        <c:crossAx val="608992112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7747,7 +7725,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7854,7 +7831,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7955,7 +7931,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -8099,7 +8074,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -8189,11 +8163,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="565290704"/>
-        <c:axId val="565289920"/>
+        <c:axId val="609000736"/>
+        <c:axId val="608998776"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="565290704"/>
+        <c:axId val="609000736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8236,7 +8210,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="565289920"/>
+        <c:crossAx val="608998776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8244,7 +8218,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="565289920"/>
+        <c:axId val="608998776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8295,7 +8269,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="565290704"/>
+        <c:crossAx val="609000736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8309,7 +8283,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -16011,15 +15984,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>573741</xdr:colOff>
+      <xdr:colOff>562856</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>8965</xdr:rowOff>
+      <xdr:rowOff>43542</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>143434</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>62753</xdr:rowOff>
+      <xdr:colOff>132549</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -16041,15 +16014,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>116541</xdr:colOff>
+      <xdr:colOff>127428</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>295834</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>53788</xdr:rowOff>
+      <xdr:colOff>306721</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>65314</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -16080,8 +16053,8 @@
     <xdr:to>
       <xdr:col>22</xdr:col>
       <xdr:colOff>376516</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>53788</xdr:rowOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -16105,15 +16078,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>591670</xdr:colOff>
+      <xdr:colOff>559013</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>53790</xdr:rowOff>
+      <xdr:rowOff>75561</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>161363</xdr:colOff>
+      <xdr:colOff>128706</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>107578</xdr:rowOff>
+      <xdr:rowOff>129349</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -16137,15 +16110,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>116541</xdr:colOff>
+      <xdr:colOff>127426</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>62753</xdr:rowOff>
+      <xdr:rowOff>51867</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>295834</xdr:colOff>
+      <xdr:colOff>306719</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>116541</xdr:rowOff>
+      <xdr:rowOff>105655</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -16169,15 +16142,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>197223</xdr:colOff>
+      <xdr:colOff>306079</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>71715</xdr:rowOff>
+      <xdr:rowOff>49943</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>376516</xdr:colOff>
+      <xdr:colOff>485372</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>125503</xdr:rowOff>
+      <xdr:rowOff>103731</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -16200,16 +16173,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>62753</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>607039</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>98611</xdr:rowOff>
+      <xdr:rowOff>141514</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>242046</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:colOff>176732</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>10886</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -16731,7 +16704,7 @@
   <dimension ref="A1:U43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AD18" sqref="AD18"/>
+      <selection activeCell="O37" sqref="O37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16800,40 +16773,40 @@
         <v>0.67</v>
       </c>
       <c r="F2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>0.56000000000000005</v>
+        <v>0.5</v>
       </c>
       <c r="I2">
-        <v>0.76</v>
+        <v>0.67</v>
       </c>
       <c r="L2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M2">
         <v>2</v>
       </c>
       <c r="N2">
-        <v>0.47</v>
+        <v>0.46</v>
       </c>
       <c r="O2">
-        <v>0.81</v>
+        <v>0.79</v>
       </c>
       <c r="R2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="S2">
         <v>3</v>
       </c>
       <c r="T2">
-        <v>0.5</v>
+        <v>0.44</v>
       </c>
       <c r="U2">
-        <v>0.76</v>
+        <v>0.77</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
@@ -16850,40 +16823,40 @@
         <v>0.79</v>
       </c>
       <c r="F3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>0.44</v>
+        <v>0.5</v>
       </c>
       <c r="I3">
-        <v>0.6</v>
+        <v>0.68</v>
       </c>
       <c r="L3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M3">
         <v>2</v>
       </c>
       <c r="N3">
-        <v>0.46</v>
+        <v>0.48</v>
       </c>
       <c r="O3">
-        <v>0.84</v>
+        <v>0.77</v>
       </c>
       <c r="R3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="S3">
         <v>3</v>
       </c>
       <c r="T3">
-        <v>0.43</v>
+        <v>0.46</v>
       </c>
       <c r="U3">
-        <v>0.75</v>
+        <v>0.76</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
@@ -16900,31 +16873,31 @@
         <v>0.77</v>
       </c>
       <c r="F4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G4">
         <v>1</v>
       </c>
       <c r="H4">
-        <v>0.44</v>
+        <v>0.53</v>
       </c>
       <c r="I4">
-        <v>0.6</v>
+        <v>0.75</v>
       </c>
       <c r="L4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M4">
         <v>2</v>
       </c>
       <c r="N4">
-        <v>0.52</v>
+        <v>0.47</v>
       </c>
       <c r="O4">
-        <v>0.79</v>
+        <v>0.77</v>
       </c>
       <c r="R4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="S4">
         <v>3</v>
@@ -16933,7 +16906,7 @@
         <v>0.47</v>
       </c>
       <c r="U4">
-        <v>0.73</v>
+        <v>0.76</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.3">
@@ -16950,40 +16923,40 @@
         <v>0.82</v>
       </c>
       <c r="F5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G5">
         <v>1</v>
       </c>
       <c r="H5">
-        <v>0.56999999999999995</v>
+        <v>0.5</v>
       </c>
       <c r="I5">
-        <v>0.79</v>
+        <v>0.67</v>
       </c>
       <c r="L5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M5">
         <v>2</v>
       </c>
       <c r="N5">
-        <v>0.54</v>
+        <v>0.47</v>
       </c>
       <c r="O5">
-        <v>0.79</v>
+        <v>0.75</v>
       </c>
       <c r="R5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="S5">
         <v>3</v>
       </c>
       <c r="T5">
-        <v>0.48</v>
+        <v>0.45</v>
       </c>
       <c r="U5">
-        <v>0.73</v>
+        <v>0.77</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.3">
@@ -17000,40 +16973,40 @@
         <v>0.8</v>
       </c>
       <c r="F6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G6">
         <v>1</v>
       </c>
       <c r="H6">
-        <v>0.43</v>
+        <v>0.52</v>
       </c>
       <c r="I6">
-        <v>0.6</v>
+        <v>0.77</v>
       </c>
       <c r="L6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="M6">
         <v>2</v>
       </c>
       <c r="N6">
-        <v>0.43</v>
+        <v>0.49</v>
       </c>
       <c r="O6">
-        <v>0.77</v>
+        <v>0.74</v>
       </c>
       <c r="R6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="S6">
         <v>3</v>
       </c>
       <c r="T6">
-        <v>0.42</v>
+        <v>0.46</v>
       </c>
       <c r="U6">
-        <v>0.74</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.3">
@@ -17050,19 +17023,19 @@
         <v>0.78</v>
       </c>
       <c r="F7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G7">
         <v>1</v>
       </c>
       <c r="H7">
-        <v>0.47</v>
+        <v>0.52</v>
       </c>
       <c r="I7">
-        <v>0.68</v>
+        <v>0.75</v>
       </c>
       <c r="L7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="M7">
         <v>2</v>
@@ -17071,19 +17044,19 @@
         <v>0.49</v>
       </c>
       <c r="O7">
-        <v>0.73</v>
+        <v>0.76</v>
       </c>
       <c r="R7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="S7">
         <v>3</v>
       </c>
       <c r="T7">
-        <v>0.48</v>
+        <v>0.46</v>
       </c>
       <c r="U7">
-        <v>0.72</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.3">
@@ -17304,31 +17277,31 @@
         <v>0.79</v>
       </c>
       <c r="F20" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G20">
         <v>4</v>
       </c>
       <c r="H20">
-        <v>0.46</v>
+        <v>0.45</v>
       </c>
       <c r="I20">
-        <v>0.81</v>
+        <v>0.82</v>
       </c>
       <c r="L20" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M20">
         <v>6</v>
       </c>
       <c r="N20">
-        <v>0.53</v>
+        <v>0.47</v>
       </c>
       <c r="O20">
-        <v>0.79</v>
+        <v>0.8</v>
       </c>
       <c r="R20" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="S20">
         <v>8</v>
@@ -17354,40 +17327,40 @@
         <v>0.79</v>
       </c>
       <c r="F21" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G21">
         <v>4</v>
       </c>
       <c r="H21">
-        <v>0.45</v>
+        <v>0.46</v>
       </c>
       <c r="I21">
-        <v>0.82</v>
+        <v>0.81</v>
       </c>
       <c r="L21" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M21">
         <v>6</v>
       </c>
       <c r="N21">
-        <v>0.44</v>
+        <v>0.48</v>
       </c>
       <c r="O21">
-        <v>0.78</v>
+        <v>0.79</v>
       </c>
       <c r="R21" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="S21">
         <v>8</v>
       </c>
       <c r="T21">
-        <v>0.44</v>
+        <v>0.43</v>
       </c>
       <c r="U21">
-        <v>0.78</v>
+        <v>0.77</v>
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.3">
@@ -17404,40 +17377,40 @@
         <v>0.81</v>
       </c>
       <c r="F22" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G22">
         <v>4</v>
       </c>
       <c r="H22">
-        <v>0.47</v>
+        <v>0.45</v>
       </c>
       <c r="I22">
-        <v>0.8</v>
+        <v>0.82</v>
       </c>
       <c r="L22" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M22">
         <v>6</v>
       </c>
       <c r="N22">
-        <v>0.51</v>
+        <v>0.46</v>
       </c>
       <c r="O22">
-        <v>0.77</v>
+        <v>0.79</v>
       </c>
       <c r="R22" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="S22">
         <v>8</v>
       </c>
       <c r="T22">
-        <v>0.43</v>
+        <v>0.44</v>
       </c>
       <c r="U22">
-        <v>0.76</v>
+        <v>0.79</v>
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.3">
@@ -17454,40 +17427,40 @@
         <v>0.67</v>
       </c>
       <c r="F23" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G23">
         <v>4</v>
       </c>
       <c r="H23">
-        <v>0.46</v>
+        <v>0.45</v>
       </c>
       <c r="I23">
-        <v>0.8</v>
+        <v>0.83</v>
       </c>
       <c r="L23" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M23">
         <v>6</v>
       </c>
       <c r="N23">
-        <v>0.5</v>
+        <v>0.44</v>
       </c>
       <c r="O23">
-        <v>0.78</v>
+        <v>0.79</v>
       </c>
       <c r="R23" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="S23">
         <v>8</v>
       </c>
       <c r="T23">
-        <v>0.43</v>
+        <v>0.44</v>
       </c>
       <c r="U23">
-        <v>0.76</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.3">
@@ -17504,7 +17477,7 @@
         <v>0.75</v>
       </c>
       <c r="F24" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G24">
         <v>4</v>
@@ -17516,19 +17489,19 @@
         <v>0.82</v>
       </c>
       <c r="L24" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="M24">
         <v>6</v>
       </c>
       <c r="N24">
-        <v>0.44</v>
+        <v>0.52</v>
       </c>
       <c r="O24">
-        <v>0.78</v>
+        <v>0.79</v>
       </c>
       <c r="R24" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="S24">
         <v>8</v>
@@ -17554,40 +17527,40 @@
         <v>0.77</v>
       </c>
       <c r="F25" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G25">
         <v>4</v>
       </c>
       <c r="H25">
-        <v>0.45</v>
+        <v>0.46</v>
       </c>
       <c r="I25">
-        <v>0.8</v>
+        <v>0.82</v>
       </c>
       <c r="L25" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="M25">
         <v>6</v>
       </c>
       <c r="N25">
-        <v>0.56999999999999995</v>
+        <v>0.49</v>
       </c>
       <c r="O25">
         <v>0.79</v>
       </c>
       <c r="R25" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="S25">
         <v>8</v>
       </c>
       <c r="T25">
-        <v>0.43</v>
+        <v>0.44</v>
       </c>
       <c r="U25">
-        <v>0.76</v>
+        <v>0.79</v>
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.3">
@@ -17714,16 +17687,16 @@
         <v>0.82</v>
       </c>
       <c r="F33" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G33">
         <v>10</v>
       </c>
       <c r="H33">
-        <v>0.42</v>
+        <v>0.45</v>
       </c>
       <c r="I33">
-        <v>0.71</v>
+        <v>0.81</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
@@ -17740,16 +17713,16 @@
         <v>0.79</v>
       </c>
       <c r="F34" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G34">
         <v>10</v>
       </c>
       <c r="H34">
-        <v>0.42</v>
+        <v>0.44</v>
       </c>
       <c r="I34">
-        <v>0.71</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
@@ -17766,16 +17739,16 @@
         <v>0.78</v>
       </c>
       <c r="F35" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G35">
         <v>10</v>
       </c>
       <c r="H35">
-        <v>0.42</v>
+        <v>0.45</v>
       </c>
       <c r="I35">
-        <v>0.71</v>
+        <v>0.81</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
@@ -17792,16 +17765,16 @@
         <v>0.8</v>
       </c>
       <c r="F36" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G36">
         <v>10</v>
       </c>
       <c r="H36">
-        <v>0.42</v>
+        <v>0.44</v>
       </c>
       <c r="I36">
-        <v>0.71</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
@@ -17818,16 +17791,16 @@
         <v>0.75</v>
       </c>
       <c r="F37" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G37">
         <v>10</v>
       </c>
       <c r="H37">
-        <v>0.42</v>
+        <v>0.44</v>
       </c>
       <c r="I37">
-        <v>0.71</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
@@ -17844,16 +17817,16 @@
         <v>0.76</v>
       </c>
       <c r="F38" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G38">
         <v>10</v>
       </c>
       <c r="H38">
-        <v>0.42</v>
+        <v>0.44</v>
       </c>
       <c r="I38">
-        <v>0.71</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Majority voter class written and implemented for veracity performance testing
</commit_message>
<xml_diff>
--- a/src/performance_testing/dastpheme_performance.xlsx
+++ b/src/performance_testing/dastpheme_performance.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9372"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9372" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="NOT_UPDATED" sheetId="4" r:id="rId1"/>
@@ -977,11 +977,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="608985448"/>
-        <c:axId val="608989368"/>
+        <c:axId val="578865016"/>
+        <c:axId val="578865408"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="608985448"/>
+        <c:axId val="578865016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1024,7 +1024,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="608989368"/>
+        <c:crossAx val="578865408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1032,7 +1032,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="608989368"/>
+        <c:axId val="578865408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1083,7 +1083,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="608985448"/>
+        <c:crossAx val="578865016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1204,6 +1204,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1304,6 +1305,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1447,6 +1449,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1536,11 +1539,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="609002696"/>
-        <c:axId val="609003088"/>
+        <c:axId val="578837648"/>
+        <c:axId val="578844704"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="609002696"/>
+        <c:axId val="578837648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1583,7 +1586,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="609003088"/>
+        <c:crossAx val="578844704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1591,7 +1594,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="609003088"/>
+        <c:axId val="578844704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1642,7 +1645,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="609002696"/>
+        <c:crossAx val="578837648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1656,6 +1659,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1762,6 +1766,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1862,6 +1867,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2005,6 +2011,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2094,11 +2101,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="609004264"/>
-        <c:axId val="609001128"/>
+        <c:axId val="578846664"/>
+        <c:axId val="578841568"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="609004264"/>
+        <c:axId val="578846664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2141,7 +2148,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="609001128"/>
+        <c:crossAx val="578841568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2149,7 +2156,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="609001128"/>
+        <c:axId val="578841568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2200,7 +2207,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="609004264"/>
+        <c:crossAx val="578846664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2214,6 +2221,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2320,6 +2328,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2420,6 +2429,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2563,6 +2573,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2652,11 +2663,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="609001520"/>
-        <c:axId val="609002304"/>
+        <c:axId val="578839216"/>
+        <c:axId val="578839608"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="609001520"/>
+        <c:axId val="578839216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2699,7 +2710,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="609002304"/>
+        <c:crossAx val="578839608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2707,7 +2718,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="609002304"/>
+        <c:axId val="578839608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2758,7 +2769,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="609001520"/>
+        <c:crossAx val="578839216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2772,6 +2783,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2878,6 +2890,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2978,6 +2991,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -3121,6 +3135,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -3210,11 +3225,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="608997992"/>
-        <c:axId val="608999560"/>
+        <c:axId val="437661456"/>
+        <c:axId val="437657928"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="608997992"/>
+        <c:axId val="437661456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3257,7 +3272,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="608999560"/>
+        <c:crossAx val="437657928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3265,7 +3280,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="608999560"/>
+        <c:axId val="437657928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3316,7 +3331,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="608997992"/>
+        <c:crossAx val="437661456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3330,6 +3345,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3481,6 +3497,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -3617,6 +3634,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -3699,11 +3717,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="609001912"/>
-        <c:axId val="608999952"/>
+        <c:axId val="437658320"/>
+        <c:axId val="437661848"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="609001912"/>
+        <c:axId val="437658320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3746,7 +3764,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="608999952"/>
+        <c:crossAx val="437661848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3754,7 +3772,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="608999952"/>
+        <c:axId val="437661848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3805,7 +3823,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="609001912"/>
+        <c:crossAx val="437658320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3819,6 +3837,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4256,11 +4275,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="608990544"/>
-        <c:axId val="608992896"/>
+        <c:axId val="578864624"/>
+        <c:axId val="578866192"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="608990544"/>
+        <c:axId val="578864624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4303,7 +4322,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="608992896"/>
+        <c:crossAx val="578866192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4311,7 +4330,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="608992896"/>
+        <c:axId val="578866192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4362,7 +4381,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="608990544"/>
+        <c:crossAx val="578864624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4814,11 +4833,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="608995640"/>
-        <c:axId val="608988976"/>
+        <c:axId val="578866584"/>
+        <c:axId val="578863448"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="608995640"/>
+        <c:axId val="578866584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4861,7 +4880,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="608988976"/>
+        <c:crossAx val="578863448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4869,7 +4888,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="608988976"/>
+        <c:axId val="578863448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4920,7 +4939,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="608995640"/>
+        <c:crossAx val="578866584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5372,11 +5391,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="608994856"/>
-        <c:axId val="608994072"/>
+        <c:axId val="578847448"/>
+        <c:axId val="578847840"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="608994856"/>
+        <c:axId val="578847448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5419,7 +5438,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="608994072"/>
+        <c:crossAx val="578847840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5427,7 +5446,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="608994072"/>
+        <c:axId val="578847840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5478,7 +5497,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="608994856"/>
+        <c:crossAx val="578847448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5930,11 +5949,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="608997600"/>
-        <c:axId val="608986232"/>
+        <c:axId val="578848232"/>
+        <c:axId val="578849016"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="608997600"/>
+        <c:axId val="578848232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5977,7 +5996,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="608986232"/>
+        <c:crossAx val="578849016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5985,7 +6004,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="608986232"/>
+        <c:axId val="578849016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6036,7 +6055,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="608997600"/>
+        <c:crossAx val="578848232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6488,11 +6507,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="608986624"/>
-        <c:axId val="608987016"/>
+        <c:axId val="578836472"/>
+        <c:axId val="578834904"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="608986624"/>
+        <c:axId val="578836472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6535,7 +6554,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="608987016"/>
+        <c:crossAx val="578834904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6543,7 +6562,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="608987016"/>
+        <c:axId val="578834904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6594,7 +6613,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="608986624"/>
+        <c:crossAx val="578836472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7046,11 +7065,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="608987408"/>
-        <c:axId val="608997208"/>
+        <c:axId val="578843920"/>
+        <c:axId val="578836864"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="608987408"/>
+        <c:axId val="578843920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7093,7 +7112,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="608997208"/>
+        <c:crossAx val="578836864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7101,7 +7120,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="608997208"/>
+        <c:axId val="578836864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7152,7 +7171,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="608987408"/>
+        <c:crossAx val="578843920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7273,6 +7292,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7373,6 +7393,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -7516,6 +7537,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -7605,11 +7627,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="608992112"/>
-        <c:axId val="608988192"/>
+        <c:axId val="578835688"/>
+        <c:axId val="578841176"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="608992112"/>
+        <c:axId val="578835688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7652,7 +7674,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="608988192"/>
+        <c:crossAx val="578841176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7660,7 +7682,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="608988192"/>
+        <c:axId val="578841176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7711,7 +7733,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="608992112"/>
+        <c:crossAx val="578835688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7725,6 +7747,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7831,6 +7854,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7931,6 +7955,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -8074,6 +8099,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -8163,11 +8189,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="609000736"/>
-        <c:axId val="608998776"/>
+        <c:axId val="578845880"/>
+        <c:axId val="578837256"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="609000736"/>
+        <c:axId val="578845880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8210,7 +8236,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="608998776"/>
+        <c:crossAx val="578837256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8218,7 +8244,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="608998776"/>
+        <c:axId val="578837256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8269,7 +8295,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="609000736"/>
+        <c:crossAx val="578845880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8283,6 +8309,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -16703,7 +16730,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="O37" sqref="O37"/>
     </sheetView>
   </sheetViews>
@@ -18532,7 +18559,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="R8" sqref="R8"/>
     </sheetView>
   </sheetViews>

</xml_diff>